<commit_message>
Experience & sidewide cosmetics (incl. webcard)
</commit_message>
<xml_diff>
--- a/files/CR_Publications.xlsx
+++ b/files/CR_Publications.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rauh\Nextcloud\WZB_CR\Datensaetze\ChRauh.github.io\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rauh\NextCloudSync\WZB_CR\Datensaetze\ChRauh.github.io\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E1A579-83D8-4C19-9E09-205C4D9FFFED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18692716-084C-4DE6-B6F0-FC20E17F189D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="580">
   <si>
     <t>Cites</t>
   </si>
@@ -1105,9 +1105,6 @@
     <t>**Undermining, defusing or defending European integration? Assessing public communication of European executives in times of EU politicisation**</t>
   </si>
   <si>
-    <t>**Authority, politicization, and alternative justifications: endogenous legitimation dynamics in global economic governance1**</t>
-  </si>
-  <si>
     <t>**Christina J. Schneider. 2018. The Responsive Union: National Elections and European Governance.(Cambridge: Cambridge University Press)**</t>
   </si>
   <si>
@@ -1168,9 +1165,6 @@
     <t>**Which policy for Europe?: Power and Conflict inside the European Commission**</t>
   </si>
   <si>
-    <t>Jan Schwalbach, L Hetzer, Sven Oliver Proksch, &lt;u&gt;Christian Rauh&lt;/u&gt;, Miklos Sebők</t>
-  </si>
-  <si>
     <t>&lt;u&gt;Christian Rauh&lt;/u&gt;, Jan Schwalbach</t>
   </si>
   <si>
@@ -1631,13 +1625,148 @@
   </si>
   <si>
     <t>https://bibliothek.wzb.eu/artikel/2024/f-26064.pdf</t>
+  </si>
+  <si>
+    <t>**Autorität ohne Rückhalt: Das Legitimationsdefizit internationaler Organisationen**</t>
+  </si>
+  <si>
+    <t>2020-03-15</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>167: 10-12</t>
+  </si>
+  <si>
+    <t>https://bibliothek.wzb.eu/artikel/2020/f-22763.pdf</t>
+  </si>
+  <si>
+    <t>**Untergraben, verschleiern, verteidigen: Politische Kommunikation zur Europäischen Union**</t>
+  </si>
+  <si>
+    <t>2019-09-15</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>165: 34-35</t>
+  </si>
+  <si>
+    <t>https://bibliothek.wzb.eu/artikel/2019/f-22368.pdf</t>
+  </si>
+  <si>
+    <t>**Legitimität und Politisierung globaler Steuerung**</t>
+  </si>
+  <si>
+    <t>2015-04-15</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>Informationen zur politischen Bildung (izpb)</t>
+  </si>
+  <si>
+    <t>325: 25-28</t>
+  </si>
+  <si>
+    <t>https://www.bpb.de/shop/zeitschriften/izpb/regieren-jenseits-des-nationalstaates-325/204681/legitimitaet-und-politisierung-globaler-steuerung/</t>
+  </si>
+  <si>
+    <t>**Und sie hört doch hin – manchmal: Öffentliche Debatten können die Politik der EU-Kommission beeinflussen**</t>
+  </si>
+  <si>
+    <t>2013-03-15</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>139: 29-31</t>
+  </si>
+  <si>
+    <t>https://bibliothek.wzb.eu/artikel/2013/f-17763.pdf</t>
+  </si>
+  <si>
+    <t>**Politisieren lassen oder politisieren? Die europäische Öffentlichkeit fordert ihr Recht**</t>
+  </si>
+  <si>
+    <t>Neue Gesellschaft/Frankfurter Hefte</t>
+  </si>
+  <si>
+    <t>60 (1/2): 53-6</t>
+  </si>
+  <si>
+    <t>https://www.frankfurter-hefte.de/artikel/die-europaeische-oeffentlichkeit-fordert-ihr-recht-1300/</t>
+  </si>
+  <si>
+    <t>https://www.frankfurter-hefte.de/media/Archiv/2013/Heft_01-02/2013-01-02_rauh.pdf</t>
+  </si>
+  <si>
+    <t>**Über den Tellerrand: Zunehmend werden auch die Entscheidungen internationaler Institutionen öffentlich politisiert**</t>
+  </si>
+  <si>
+    <t>2013-09-15</t>
+  </si>
+  <si>
+    <t>141: 31-23</t>
+  </si>
+  <si>
+    <t>https://bibliothek.wzb.eu/artikel/2013/f-18061.pdf</t>
+  </si>
+  <si>
+    <t>**Klarer über Europa reden. warum europäische Entscheidungsträger ihre Kommunikation verbessern müssen**</t>
+  </si>
+  <si>
+    <t>2023-03-13</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>179: Online Supplement</t>
+  </si>
+  <si>
+    <t>https://bibliothek.wzb.eu/artikel/2023/f-25373.pdf</t>
+  </si>
+  <si>
+    <t>https://www.wzb.eu/de/artikel/klarer-ueber-europa-reden</t>
+  </si>
+  <si>
+    <t>**Eine Frage des Vertrauens: Warum Menschen die Corona-Impfung ablehnen**</t>
+  </si>
+  <si>
+    <t>2022-03-15</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>Jan Paul Heisig, Heiko Giebler, &lt;u&gt;Christian Rauh&lt;/u&gt;</t>
+  </si>
+  <si>
+    <t>175: 36-39</t>
+  </si>
+  <si>
+    <t>https://bibliothek.wzb.eu/artikel/2022/f-24610.pdf</t>
+  </si>
+  <si>
+    <t>https://www.wzb.eu/de/publikationen/wzb-mitteilungen/nr-175-gesundheit</t>
+  </si>
+  <si>
+    <t>**Authority, politicization, and alternative justifications: endogenous legitimation dynamics in global economic governance**</t>
+  </si>
+  <si>
+    <t>Jan Schwalbach, Lukas Hetzer, Sven Oliver Proksch, &lt;u&gt;Christian Rauh&lt;/u&gt;, Miklos Sebők</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1768,6 +1897,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2070,7 +2207,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2113,8 +2250,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2129,8 +2267,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2161,6 +2301,7 @@
     <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
@@ -2238,6 +2379,798 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{307FFD5D-ACC8-4D26-8637-0C20E892C117}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="11430000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC1DE0B8-4D4B-461D-BD67-9C99B886BDB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="11620500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C835908-C0CD-4690-BF76-5B132FAB5D93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="11811000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F36A0332-E27C-4EF7-BE2B-8C960376D100}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="11811000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46376E4A-2BBD-4CC6-9C28-6C408F4581DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12001500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAACD8BD-8B28-4F92-8AB8-0CC854F180A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12192000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8CF7F78-AF9E-4540-957A-5B48F796D651}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12382500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E33AB15D-18C9-45BC-9E9E-DEC6ADEC5FF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12192000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14611F73-953F-498D-9CA6-812413C820F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12382500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D9A7C6F-CBAD-4B9A-AE51-1FAD05BB61BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12382500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9C623B3-B636-440F-A572-B376DADB2355}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12192000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B4E048C-EB61-4A13-B529-F5A2E8664D37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12382500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{392E5A51-D84F-4BEB-94F1-8B51845D387B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12382500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{242C2D5E-22C3-4BE8-AF04-E85B2928047C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12573000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E994FBE7-21E9-4954-920A-78C9F1CBBE53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12573000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA579032-F9D6-44C2-B128-CD76B4D9BBD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12763500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0E5042E-EBEB-4069-8085-21239885BCE3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12763500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="AutoShape 3" descr="data:image/svg+xml;base64,PD94bWwgdmVyc2lvbj0iMS4wIiBlbmNvZGluZz0idXRmLTgiPz48IURPQ1RZUEUgc3ZnIFBVQkxJQyAiLS8vVzNDLy9EVEQgU1ZHIDEuMS8vRU4iICJodHRwOi8vd3d3LnczLm9yZy9HcmFwaGljcy9TVkcvMS4xL0RURC9zdmcxMS5kdGQiPjxzdmcgdmVyc2lvbj0iMS4xIiBpZD0iRWJlbmVfMSIgeG1sbnM9Imh0dHA6Ly93d3cudzMub3JnLzIwMDAvc3ZnIiB4bWxuczp4bGluaz0iaHR0cDovL3d3dy53My5vcmcvMTk5OS94bGluayIgeD0iMHB4IiB5PSIwcHgiIHdpZHRoPSIxNnB4IiBoZWlnaHQ9IjE2cHgiIHZpZXdCb3g9IjAgMCAxNiAxNiIgZW5hYmxlLWJhY2tncm91bmQ9Im5ldyAwIDAgMTYgMTYiIHhtbDpzcGFjZT0icHJlc2VydmUiPjxnPjxnPjxwYXRoIGZpbGw9IiNGRkZGRkYiIGQ9Ik04LjAwMSwxNS41QzMuODY0LDE1LjUsMC41LDEyLjEzNiwwLjUsOGMwLTQuMTM1LDMuMzY1LTcuNSw3LjUwMS03LjVTMTUuNSwzLjg2NCwxNS41LDhTMTIuMTM3LDE1LjUsOC4wMDEsMTUuNXoiLz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNOC4wMDEsMUMxMS44NiwxLDE1LDQuMTQxLDE1LDhzLTMuMTM5LDctNi45OTksN0M0LjE0LDE1LDEsMTEuODU5LDEsOFM0LjE0LDEsOC4wMDEsMSBNOC4wMDEsMEMzLjU4MiwwLDAsMy41ODIsMCw4czMuNTgyLDgsOC4wMDEsOEMxMi40MTgsMTYsMTYsMTIuNDE4LDE2LDhTMTIuNDE4LDAsOC4wMDEsMEw4LjAwMSwweiIvPjwvZz48cGF0aCBmaWxsPSIjRDUyQjFFIiBkPSJNNi43NDUsMTIuNTg5Yy0wLjIyNywwLjEyMi0wLjQ5NywwLjI0Ny0wLjY4NCwwLjI0N2MtMC4zMTgsMC0wLjUwMS0wLjE2NC0wLjUwMS0wLjQ1MmMwLTAuMjA3LDAuMTQtMC4zNzUsMC41OTUtMC42MjJjMS41NDktMC45MDQsMi41OTQtMi4yNzIsMi41OTQtMy43MjFjMC0wLjgyNS0wLjIyNy0xLjExOS0wLjY4MS0xLjExOWMtMC4xMzUsMC0wLjMyLDAuMjE5LTAuNjM2LDAuMjE5SDcuMTU3QzYuMTAyLDcuMTQzLDUuMzMzLDYuMjY0LDUuMzMzLDUuMjNjMC0xLjE1MiwwLjk1OC0yLjAwNiwyLjI4LTIuMDA2YzEuNzc3LDAsMy4wNTMsMS4zNzMsMy4wNTMsMy40M0MxMC42NjYsOS4yMTUsOS4yMDMsMTEuMjcsNi43NDUsMTIuNTg5Ii8+PC9nPjwvc3ZnPg">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D705CA1-B85C-4224-B3FC-41600F8061FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11239500" y="12763500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2539,25 +3472,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:AI62"/>
+  <dimension ref="A1:AI70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A62" sqref="A62"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="6" max="7" width="11.5546875" style="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
-    <col min="12" max="12" width="11.5546875" style="2"/>
-    <col min="13" max="13" width="11.44140625" style="2"/>
+    <col min="6" max="7" width="11.5703125" style="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="2"/>
+    <col min="13" max="13" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>152</v>
       </c>
@@ -2595,7 +3528,7 @@
         <v>164</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>165</v>
@@ -2664,7 +3597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>153</v>
       </c>
@@ -2685,17 +3618,17 @@
         <v>2025</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>382</v>
+        <v>579</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>146</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="K2" s="2"/>
       <c r="N2" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>144</v>
@@ -2704,13 +3637,13 @@
         <v>214</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -2743,7 +3676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>153</v>
       </c>
@@ -2764,13 +3697,13 @@
         <v>2022</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>111</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="K3" s="2"/>
       <c r="N3" s="2"/>
@@ -2781,13 +3714,13 @@
         <v>203</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -2818,7 +3751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>153</v>
       </c>
@@ -2841,7 +3774,7 @@
         <v>2022</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>147</v>
@@ -2861,13 +3794,13 @@
         <v>215</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>324</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
@@ -2906,7 +3839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>153</v>
       </c>
@@ -2927,7 +3860,7 @@
         <v>2020</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>26</v>
@@ -2952,7 +3885,7 @@
         <v>320</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
@@ -2987,7 +3920,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>153</v>
       </c>
@@ -3008,13 +3941,13 @@
         <v>2018</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="K6" s="2"/>
       <c r="N6" s="2"/>
@@ -3025,11 +3958,11 @@
         <v>197</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
@@ -3060,7 +3993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>153</v>
       </c>
@@ -3081,7 +4014,7 @@
         <v>2017</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>69</v>
@@ -3106,7 +4039,7 @@
         <v>319</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
@@ -3139,7 +4072,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>153</v>
       </c>
@@ -3160,7 +4093,7 @@
         <v>2016</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>19</v>
@@ -3177,11 +4110,11 @@
         <v>210</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
@@ -3212,7 +4145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>153</v>
       </c>
@@ -3233,7 +4166,7 @@
         <v>2015</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>14</v>
@@ -3250,11 +4183,11 @@
         <v>217</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
@@ -3285,7 +4218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>153</v>
       </c>
@@ -3306,17 +4239,17 @@
         <v>2015</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>105</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
@@ -3326,11 +4259,11 @@
         <v>201</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
@@ -3365,7 +4298,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>153</v>
       </c>
@@ -3386,7 +4319,7 @@
         <v>2014</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>19</v>
@@ -3403,11 +4336,11 @@
         <v>218</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -3438,7 +4371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>153</v>
       </c>
@@ -3459,17 +4392,17 @@
         <v>2014</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2" t="s">
@@ -3512,7 +4445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>153</v>
       </c>
@@ -3533,7 +4466,7 @@
         <v>2014</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>117</v>
@@ -3553,7 +4486,7 @@
         <v>205</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -3594,9 +4527,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>336</v>
@@ -3615,7 +4548,7 @@
         <v>2013</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>19</v>
@@ -3665,9 +4598,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>337</v>
@@ -3686,7 +4619,7 @@
         <v>2013</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>19</v>
@@ -3734,9 +4667,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>338</v>
@@ -3755,7 +4688,7 @@
         <v>2013</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>89</v>
@@ -3810,12 +4743,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
@@ -3831,7 +4764,7 @@
         <v>2012</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>19</v>
@@ -3848,7 +4781,7 @@
         <v>194</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -3881,7 +4814,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>153</v>
       </c>
@@ -3902,7 +4835,7 @@
         <v>2010</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>14</v>
@@ -3912,7 +4845,7 @@
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2" t="s">
@@ -3922,11 +4855,11 @@
         <v>207</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
@@ -3957,7 +4890,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>153</v>
       </c>
@@ -3978,7 +4911,7 @@
         <v>2010</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>14</v>
@@ -3988,7 +4921,7 @@
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2" t="s">
@@ -3998,7 +4931,7 @@
         <v>190</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -4031,7 +4964,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>153</v>
       </c>
@@ -4052,13 +4985,13 @@
         <v>2010</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2">
@@ -4072,11 +5005,11 @@
         <v>209</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
@@ -4109,9 +5042,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>342</v>
@@ -4130,7 +5063,7 @@
         <v>2009</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>19</v>
@@ -4176,7 +5109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>153</v>
       </c>
@@ -4197,7 +5130,7 @@
         <v>2009</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>19</v>
@@ -4254,9 +5187,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>344</v>
@@ -4275,7 +5208,7 @@
         <v>2008</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>14</v>
@@ -4330,7 +5263,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>153</v>
       </c>
@@ -4351,7 +5284,7 @@
         <v>2008</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>19</v>
@@ -4397,7 +5330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>153</v>
       </c>
@@ -4418,7 +5351,7 @@
         <v>2007</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>19</v>
@@ -4435,7 +5368,7 @@
         <v>221</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
@@ -4468,7 +5401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>153</v>
       </c>
@@ -4489,7 +5422,7 @@
         <v>2006</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>19</v>
@@ -4506,7 +5439,7 @@
         <v>222</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
@@ -4539,7 +5472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>153</v>
       </c>
@@ -4560,7 +5493,7 @@
         <v>2006</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>19</v>
@@ -4577,7 +5510,7 @@
         <v>223</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
@@ -4610,7 +5543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>153</v>
       </c>
@@ -4631,7 +5564,7 @@
         <v>2006</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>151</v>
@@ -4648,7 +5581,7 @@
         <v>224</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
@@ -4681,7 +5614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>153</v>
       </c>
@@ -4702,7 +5635,7 @@
         <v>2005</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>19</v>
@@ -4719,7 +5652,7 @@
         <v>212</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
@@ -4752,7 +5685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>153</v>
       </c>
@@ -4773,7 +5706,7 @@
         <v>2005</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>19</v>
@@ -4790,7 +5723,7 @@
         <v>225</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
@@ -4823,7 +5756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -4846,7 +5779,7 @@
         <v>2025</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>19</v>
@@ -4856,7 +5789,7 @@
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="N31" s="7" t="s">
         <v>298</v>
@@ -4874,7 +5807,7 @@
         <v>299</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
@@ -4909,7 +5842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -4932,7 +5865,7 @@
         <v>2025</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>58</v>
@@ -4999,7 +5932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
@@ -5022,7 +5955,7 @@
         <v>2024</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>55</v>
@@ -5044,13 +5977,13 @@
         <v>182</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="R33" s="2" t="s">
         <v>315</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
@@ -5089,7 +6022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -5112,7 +6045,7 @@
         <v>2023</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>19</v>
@@ -5179,7 +6112,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>22</v>
       </c>
@@ -5202,7 +6135,7 @@
         <v>2022</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>19</v>
@@ -5269,7 +6202,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>22</v>
       </c>
@@ -5292,7 +6225,7 @@
         <v>2022</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>62</v>
@@ -5359,7 +6292,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
@@ -5382,7 +6315,7 @@
         <v>2021</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>19</v>
@@ -5449,7 +6382,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
@@ -5472,7 +6405,7 @@
         <v>2020</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>33</v>
@@ -5485,7 +6418,7 @@
         <v>230</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="O38" s="2" t="s">
         <v>35</v>
@@ -5494,13 +6427,13 @@
         <v>173</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="R38" s="7" t="s">
         <v>317</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
@@ -5539,12 +6472,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>361</v>
+        <v>578</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>290</v>
@@ -5562,7 +6495,7 @@
         <v>2020</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>43</v>
@@ -5575,7 +6508,7 @@
         <v>232</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="O39" s="2" t="s">
         <v>45</v>
@@ -5584,13 +6517,13 @@
         <v>176</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="R39" s="2" t="s">
         <v>316</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
@@ -5629,12 +6562,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
@@ -5650,7 +6583,7 @@
         <v>2020</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>19</v>
@@ -5663,7 +6596,7 @@
         <v>247</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="O40" s="2" t="s">
         <v>144</v>
@@ -5672,11 +6605,11 @@
         <v>216</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="R40" s="2"/>
       <c r="S40" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
@@ -5715,12 +6648,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>290</v>
@@ -5738,7 +6671,7 @@
         <v>2019</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>19</v>
@@ -5751,7 +6684,7 @@
         <v>228</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="O41" s="2" t="s">
         <v>24</v>
@@ -5760,13 +6693,13 @@
         <v>170</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
@@ -5805,12 +6738,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>290</v>
@@ -5828,7 +6761,7 @@
         <v>2019</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>65</v>
@@ -5841,7 +6774,7 @@
         <v>239</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="O42" s="2" t="s">
         <v>66</v>
@@ -5850,11 +6783,11 @@
         <v>185</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="R42" s="2"/>
       <c r="S42" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
@@ -5893,12 +6826,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>290</v>
@@ -5916,7 +6849,7 @@
         <v>2018</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>19</v>
@@ -5929,7 +6862,7 @@
         <v>229</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="O43" s="2" t="s">
         <v>31</v>
@@ -5938,13 +6871,13 @@
         <v>172</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="R43" s="2" t="s">
         <v>318</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
@@ -5983,12 +6916,12 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>290</v>
@@ -6006,7 +6939,7 @@
         <v>2018</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>40</v>
@@ -6019,7 +6952,7 @@
         <v>231</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="O44" s="2" t="s">
         <v>41</v>
@@ -6028,13 +6961,13 @@
         <v>175</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
@@ -6073,12 +7006,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>290</v>
@@ -6096,7 +7029,7 @@
         <v>2016</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>67</v>
@@ -6109,7 +7042,7 @@
         <v>240</v>
       </c>
       <c r="N45" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="O45" s="2" t="s">
         <v>68</v>
@@ -6118,13 +7051,13 @@
         <v>186</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
@@ -6163,12 +7096,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>290</v>
@@ -6186,7 +7119,7 @@
         <v>2016</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>14</v>
@@ -6199,7 +7132,7 @@
         <v>243</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="O46" s="2" t="s">
         <v>109</v>
@@ -6208,11 +7141,11 @@
         <v>202</v>
       </c>
       <c r="Q46" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="R46" s="2"/>
       <c r="S46" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
@@ -6251,12 +7184,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>290</v>
@@ -6274,7 +7207,7 @@
         <v>2016</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>43</v>
@@ -6284,7 +7217,7 @@
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2" t="s">
@@ -6294,11 +7227,11 @@
         <v>193</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="R47" s="2"/>
       <c r="S47" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
@@ -6333,12 +7266,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>290</v>
@@ -6356,7 +7289,7 @@
         <v>2015</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>19</v>
@@ -6369,7 +7302,7 @@
         <v>234</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="O48" s="2" t="s">
         <v>49</v>
@@ -6378,13 +7311,13 @@
         <v>178</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
@@ -6423,12 +7356,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>290</v>
@@ -6446,7 +7379,7 @@
         <v>2013</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>98</v>
@@ -6459,7 +7392,7 @@
         <v>242</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="O49" s="2" t="s">
         <v>100</v>
@@ -6468,13 +7401,13 @@
         <v>199</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
@@ -6513,12 +7446,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>290</v>
@@ -6536,7 +7469,7 @@
         <v>2013</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>113</v>
@@ -6549,7 +7482,7 @@
         <v>244</v>
       </c>
       <c r="N50" s="7" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="O50" s="2" t="s">
         <v>115</v>
@@ -6558,11 +7491,11 @@
         <v>204</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="R50" s="2"/>
       <c r="S50" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
@@ -6601,12 +7534,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>290</v>
@@ -6624,7 +7557,7 @@
         <v>2012</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>14</v>
@@ -6634,10 +7567,10 @@
       </c>
       <c r="K51" s="2"/>
       <c r="L51" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="O51" s="2" t="s">
         <v>53</v>
@@ -6646,11 +7579,11 @@
         <v>180</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="R51" s="2"/>
       <c r="S51" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
@@ -6681,12 +7614,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>290</v>
@@ -6704,7 +7637,7 @@
         <v>2011</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>73</v>
@@ -6717,7 +7650,7 @@
         <v>241</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="O52" s="2" t="s">
         <v>75</v>
@@ -6726,11 +7659,11 @@
         <v>189</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="R52" s="2"/>
       <c r="S52" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
@@ -6769,12 +7702,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>290</v>
@@ -6792,7 +7725,7 @@
         <v>2024</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>94</v>
@@ -6805,10 +7738,10 @@
         <v>253</v>
       </c>
       <c r="M53" s="7" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="O53" s="2" t="s">
         <v>96</v>
@@ -6817,7 +7750,7 @@
         <v>198</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="R53" s="2"/>
       <c r="S53" s="2"/>
@@ -6854,12 +7787,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>290</v>
@@ -6877,7 +7810,7 @@
         <v>2021</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>19</v>
@@ -6890,10 +7823,10 @@
         <v>249</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="O54" s="2" t="s">
         <v>72</v>
@@ -6902,12 +7835,12 @@
         <v>188</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
       <c r="T54" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
@@ -6941,12 +7874,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
@@ -6962,7 +7895,7 @@
         <v>2021</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>78</v>
@@ -6975,10 +7908,10 @@
         <v>250</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="N55" s="7" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="O55" s="2" t="s">
         <v>80</v>
@@ -6987,7 +7920,7 @@
         <v>191</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
@@ -7024,12 +7957,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>290</v>
@@ -7047,7 +7980,7 @@
         <v>2017</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>81</v>
@@ -7060,7 +7993,7 @@
         <v>251</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2" t="s">
@@ -7070,12 +8003,12 @@
         <v>192</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
@@ -7111,12 +8044,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>290</v>
@@ -7134,20 +8067,20 @@
         <v>2015</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>89</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="K57" s="2"/>
       <c r="M57" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="O57" s="2" t="s">
         <v>90</v>
@@ -7156,12 +8089,12 @@
         <v>195</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
       <c r="T57" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
@@ -7191,12 +8124,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>290</v>
@@ -7214,7 +8147,7 @@
         <v>2015</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>43</v>
@@ -7227,17 +8160,17 @@
         <v>254</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="N58" s="7" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="O58" s="2" t="s">
         <v>128</v>
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" s="7" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
@@ -7274,12 +8207,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>290</v>
@@ -7297,7 +8230,7 @@
         <v>2014</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>43</v>
@@ -7310,10 +8243,10 @@
         <v>248</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="O59" s="2" t="s">
         <v>51</v>
@@ -7322,7 +8255,7 @@
         <v>179</v>
       </c>
       <c r="Q59" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
@@ -7359,12 +8292,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>290</v>
@@ -7382,7 +8315,7 @@
         <v>2016</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>19</v>
@@ -7436,12 +8369,12 @@
         <v>153</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>290</v>
@@ -7459,7 +8392,7 @@
         <v>2014</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>14</v>
@@ -7471,7 +8404,7 @@
         <v>15</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>16</v>
@@ -7515,12 +8448,12 @@
         <v>319</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
@@ -7530,13 +8463,13 @@
         <v>156</v>
       </c>
       <c r="F62" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>532</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>534</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2" t="s">
@@ -7544,17 +8477,17 @@
       </c>
       <c r="K62" s="2"/>
       <c r="L62" s="2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
       <c r="Q62" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="R62" s="2"/>
       <c r="S62" s="2" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
@@ -7573,6 +8506,470 @@
       <c r="AH62" s="2"/>
       <c r="AI62" s="2"/>
     </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="N63" s="2"/>
+      <c r="O63" s="2"/>
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="R63" s="2"/>
+      <c r="S63" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="T63" s="2"/>
+      <c r="U63" s="2"/>
+      <c r="V63" s="2"/>
+      <c r="W63" s="2"/>
+      <c r="X63" s="2"/>
+      <c r="Y63" s="2"/>
+      <c r="Z63" s="2"/>
+      <c r="AA63" s="2"/>
+      <c r="AB63" s="2"/>
+      <c r="AC63" s="2"/>
+      <c r="AD63" s="2"/>
+      <c r="AE63" s="2"/>
+      <c r="AF63" s="2"/>
+      <c r="AG63" s="2"/>
+      <c r="AH63" s="2"/>
+      <c r="AI63" s="2"/>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>541</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
+      <c r="P64" s="2"/>
+      <c r="Q64" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="R64" s="2"/>
+      <c r="S64" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="T64" s="2"/>
+      <c r="U64" s="2"/>
+      <c r="V64" s="2"/>
+      <c r="W64" s="2"/>
+      <c r="X64" s="2"/>
+      <c r="Y64" s="2"/>
+      <c r="Z64" s="2"/>
+      <c r="AA64" s="2"/>
+      <c r="AB64" s="2"/>
+      <c r="AC64" s="2"/>
+      <c r="AD64" s="2"/>
+      <c r="AE64" s="2"/>
+      <c r="AF64" s="2"/>
+      <c r="AG64" s="2"/>
+      <c r="AH64" s="2"/>
+      <c r="AI64" s="2"/>
+    </row>
+    <row r="65" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="N65" s="2"/>
+      <c r="O65" s="2"/>
+      <c r="P65" s="2"/>
+      <c r="Q65" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="R65" s="2"/>
+      <c r="S65" s="2"/>
+      <c r="T65" s="2"/>
+      <c r="U65" s="2"/>
+      <c r="V65" s="2"/>
+      <c r="W65" s="2"/>
+      <c r="X65" s="2"/>
+      <c r="Y65" s="2"/>
+      <c r="Z65" s="2"/>
+      <c r="AA65" s="2"/>
+      <c r="AB65" s="2"/>
+      <c r="AC65" s="2"/>
+      <c r="AD65" s="2"/>
+      <c r="AE65" s="2"/>
+      <c r="AF65" s="2"/>
+      <c r="AG65" s="2"/>
+      <c r="AH65" s="2"/>
+      <c r="AI65" s="2"/>
+    </row>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>552</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="N66" s="2"/>
+      <c r="O66" s="2"/>
+      <c r="P66" s="2"/>
+      <c r="Q66" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="R66" s="2"/>
+      <c r="S66" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="T66" s="2"/>
+      <c r="U66" s="2"/>
+      <c r="V66" s="2"/>
+      <c r="W66" s="2"/>
+      <c r="X66" s="2"/>
+      <c r="Y66" s="2"/>
+      <c r="Z66" s="2"/>
+      <c r="AA66" s="2"/>
+      <c r="AB66" s="2"/>
+      <c r="AC66" s="2"/>
+      <c r="AD66" s="2"/>
+      <c r="AE66" s="2"/>
+      <c r="AF66" s="2"/>
+      <c r="AG66" s="2"/>
+      <c r="AH66" s="2"/>
+      <c r="AI66" s="2"/>
+    </row>
+    <row r="67" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="I67" s="2"/>
+      <c r="J67" s="8" t="s">
+        <v>557</v>
+      </c>
+      <c r="K67" s="2"/>
+      <c r="L67" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="N67" s="2"/>
+      <c r="O67" s="2"/>
+      <c r="P67" s="2"/>
+      <c r="Q67" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="R67" s="2"/>
+      <c r="S67" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="T67" s="2"/>
+      <c r="U67" s="2"/>
+      <c r="V67" s="2"/>
+      <c r="W67" s="2"/>
+      <c r="X67" s="2"/>
+      <c r="Y67" s="2"/>
+      <c r="Z67" s="2"/>
+      <c r="AA67" s="2"/>
+      <c r="AB67" s="2"/>
+      <c r="AC67" s="2"/>
+      <c r="AD67" s="2"/>
+      <c r="AE67" s="2"/>
+      <c r="AF67" s="2"/>
+      <c r="AG67" s="2"/>
+      <c r="AH67" s="2"/>
+      <c r="AI67" s="2"/>
+    </row>
+    <row r="68" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>553</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="R68" s="2"/>
+      <c r="S68" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="T68" s="2"/>
+      <c r="U68" s="2"/>
+      <c r="V68" s="2"/>
+      <c r="W68" s="2"/>
+      <c r="X68" s="2"/>
+      <c r="Y68" s="2"/>
+      <c r="Z68" s="2"/>
+      <c r="AA68" s="2"/>
+      <c r="AB68" s="2"/>
+      <c r="AC68" s="2"/>
+      <c r="AD68" s="2"/>
+      <c r="AE68" s="2"/>
+      <c r="AF68" s="2"/>
+      <c r="AG68" s="2"/>
+      <c r="AH68" s="2"/>
+      <c r="AI68" s="2"/>
+    </row>
+    <row r="69" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>566</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>567</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="I69" s="2"/>
+      <c r="J69" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="N69" s="2"/>
+      <c r="O69" s="2"/>
+      <c r="P69" s="2"/>
+      <c r="Q69" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="R69" s="2"/>
+      <c r="S69" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="T69" s="2"/>
+      <c r="U69" s="2"/>
+      <c r="V69" s="2"/>
+      <c r="W69" s="2"/>
+      <c r="X69" s="2"/>
+      <c r="Y69" s="2"/>
+      <c r="Z69" s="2"/>
+      <c r="AA69" s="2"/>
+      <c r="AB69" s="2"/>
+      <c r="AC69" s="2"/>
+      <c r="AD69" s="2"/>
+      <c r="AE69" s="2"/>
+      <c r="AF69" s="2"/>
+      <c r="AG69" s="2"/>
+      <c r="AH69" s="2"/>
+      <c r="AI69" s="2"/>
+    </row>
+    <row r="70" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>573</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2"/>
+      <c r="P70" s="2"/>
+      <c r="Q70" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="R70" s="2"/>
+      <c r="S70" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="T70" s="2"/>
+      <c r="U70" s="2"/>
+      <c r="V70" s="2"/>
+      <c r="W70" s="2"/>
+      <c r="X70" s="2"/>
+      <c r="Y70" s="2"/>
+      <c r="Z70" s="2"/>
+      <c r="AA70" s="2"/>
+      <c r="AB70" s="2"/>
+      <c r="AC70" s="2"/>
+      <c r="AD70" s="2"/>
+      <c r="AE70" s="2"/>
+      <c r="AF70" s="2"/>
+      <c r="AG70" s="2"/>
+      <c r="AH70" s="2"/>
+      <c r="AI70" s="2"/>
+    </row>
   </sheetData>
   <sortState ref="A2:AI61">
     <sortCondition descending="1" ref="A2:A61"/>

</xml_diff>

<commit_message>
404, readme, minor cosmetics
</commit_message>
<xml_diff>
--- a/files/CR_Publications.xlsx
+++ b/files/CR_Publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rauh\NextCloudSync\WZB_CR\Datensaetze\ChRauh.github.io\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18692716-084C-4DE6-B6F0-FC20E17F189D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B378FC-4E2C-4021-A739-523AF2B95F28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="584">
   <si>
     <t>Cites</t>
   </si>
@@ -112,9 +112,6 @@
     <t>20.20</t>
   </si>
   <si>
-    <t>Journal of Information Technology &amp;Politics</t>
-  </si>
-  <si>
     <t>https://scholar.google.com/scholar?oi=bibs&amp;hl=en&amp;cites=18269512851570548391,1777725418441162154</t>
   </si>
   <si>
@@ -1760,6 +1757,21 @@
   </si>
   <si>
     <t>Jan Schwalbach, Lukas Hetzer, Sven Oliver Proksch, &lt;u&gt;Christian Rauh&lt;/u&gt;, Miklos Sebők</t>
+  </si>
+  <si>
+    <t>Journal of Information Technology &amp; Politics</t>
+  </si>
+  <si>
+    <t>289-314</t>
+  </si>
+  <si>
+    <t>doi:10.7802/2824</t>
+  </si>
+  <si>
+    <t>29-40</t>
+  </si>
+  <si>
+    <t>doi:10.7910/DVN/L4OAKN</t>
   </si>
 </sst>
 </file>
@@ -2252,7 +2264,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2269,6 +2281,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="42" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3478,7 +3491,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3492,67 +3505,67 @@
   <sheetData>
     <row r="1" spans="1:35" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>166</v>
-      </c>
       <c r="Q1" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R1" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="S1" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>261</v>
-      </c>
       <c r="U1" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>1</v>
@@ -3599,51 +3612,54 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G2" s="6">
         <v>2025</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="K2" s="2"/>
-      <c r="N2" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>470</v>
-      </c>
       <c r="S2" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -3658,7 +3674,7 @@
         <v>0</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC2" s="2">
         <v>0</v>
@@ -3678,49 +3694,52 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G3" s="6">
         <v>2022</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>582</v>
+      </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>474</v>
-      </c>
       <c r="S3" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
@@ -3733,7 +3752,7 @@
         <v>2</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AC3" s="2">
         <v>1</v>
@@ -3753,54 +3772,54 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G4" s="6">
         <v>2022</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
@@ -3821,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC4" s="2">
         <v>0</v>
@@ -3841,26 +3860,26 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G5" s="6">
         <v>2020</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>26</v>
@@ -3869,23 +3888,26 @@
         <v>27</v>
       </c>
       <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>583</v>
+      </c>
       <c r="N5" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
@@ -3922,47 +3944,47 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G6" s="6">
         <v>2018</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
@@ -3995,51 +4017,51 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G7" s="6">
         <v>2017</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="K7" s="2"/>
       <c r="N7" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
@@ -4074,47 +4096,47 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G8" s="6">
         <v>2016</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
@@ -4127,7 +4149,7 @@
         <v>1</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AC8" s="2">
         <v>1</v>
@@ -4147,47 +4169,47 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G9" s="6">
         <v>2015</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
@@ -4200,7 +4222,7 @@
         <v>0</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC9" s="2">
         <v>0</v>
@@ -4220,50 +4242,50 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G10" s="6">
         <v>2015</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
@@ -4280,7 +4302,7 @@
         <v>7</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AC10" s="2">
         <v>4</v>
@@ -4300,47 +4322,47 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G11" s="6">
         <v>2014</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
@@ -4353,7 +4375,7 @@
         <v>0</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC11" s="2">
         <v>0</v>
@@ -4373,50 +4395,50 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G12" s="6">
         <v>2014</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
@@ -4429,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC12" s="2">
         <v>0</v>
@@ -4447,46 +4469,46 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G13" s="6">
         <v>2014</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>118</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -4509,7 +4531,7 @@
         <v>4</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC13" s="2">
         <v>2</v>
@@ -4529,42 +4551,42 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G14" s="6">
         <v>2013</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K14" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -4580,7 +4602,7 @@
         <v>9</v>
       </c>
       <c r="AB14" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC14" s="2">
         <v>9</v>
@@ -4600,40 +4622,40 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G15" s="6">
         <v>2013</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -4649,7 +4671,7 @@
         <v>4</v>
       </c>
       <c r="AB15" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC15" s="2">
         <v>4</v>
@@ -4669,43 +4691,43 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G16" s="6">
         <v>2013</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -4725,7 +4747,7 @@
         <v>2</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AC16" s="2">
         <v>1</v>
@@ -4745,43 +4767,43 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G17" s="6">
         <v>2012</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -4796,7 +4818,7 @@
         <v>26</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AC17" s="2">
         <v>26</v>
@@ -4816,50 +4838,50 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G18" s="6">
         <v>2010</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
@@ -4872,7 +4894,7 @@
         <v>4</v>
       </c>
       <c r="AB18" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AC18" s="2">
         <v>1</v>
@@ -4892,46 +4914,46 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G19" s="6">
         <v>2010</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -4966,32 +4988,32 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G20" s="6">
         <v>2010</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2">
@@ -4999,17 +5021,17 @@
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
@@ -5024,7 +5046,7 @@
         <v>2</v>
       </c>
       <c r="AB20" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AC20" s="2">
         <v>1</v>
@@ -5044,26 +5066,26 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G21" s="6">
         <v>2009</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>19</v>
@@ -5072,10 +5094,10 @@
       <c r="K21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -5091,7 +5113,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC21" s="2">
         <v>0</v>
@@ -5111,43 +5133,43 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G22" s="6">
         <v>2009</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
@@ -5169,7 +5191,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC22" s="2">
         <v>0</v>
@@ -5189,43 +5211,43 @@
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G23" s="6">
         <v>2008</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
@@ -5265,26 +5287,26 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G24" s="6">
         <v>2008</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>19</v>
@@ -5293,10 +5315,10 @@
       <c r="K24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
@@ -5312,7 +5334,7 @@
         <v>1</v>
       </c>
       <c r="AB24" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AC24" s="2">
         <v>1</v>
@@ -5332,43 +5354,43 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G25" s="6">
         <v>2007</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
@@ -5383,7 +5405,7 @@
         <v>0</v>
       </c>
       <c r="AB25" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC25" s="2">
         <v>0</v>
@@ -5403,43 +5425,43 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G26" s="6">
         <v>2006</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
@@ -5454,7 +5476,7 @@
         <v>0</v>
       </c>
       <c r="AB26" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC26" s="2">
         <v>0</v>
@@ -5474,43 +5496,43 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G27" s="6">
         <v>2006</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
@@ -5525,7 +5547,7 @@
         <v>0</v>
       </c>
       <c r="AB27" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC27" s="2">
         <v>0</v>
@@ -5545,43 +5567,43 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G28" s="6">
         <v>2006</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K28" s="2"/>
       <c r="N28" s="2"/>
       <c r="O28" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
@@ -5596,7 +5618,7 @@
         <v>0</v>
       </c>
       <c r="AB28" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC28" s="2">
         <v>0</v>
@@ -5616,43 +5638,43 @@
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G29" s="6">
         <v>2005</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K29" s="2"/>
       <c r="N29" s="2"/>
       <c r="O29" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
@@ -5667,7 +5689,7 @@
         <v>1</v>
       </c>
       <c r="AB29" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AC29" s="2">
         <v>1</v>
@@ -5687,43 +5709,43 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G30" s="6">
         <v>2005</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K30" s="2"/>
       <c r="N30" s="2"/>
       <c r="O30" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
@@ -5738,7 +5760,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC30" s="2">
         <v>0</v>
@@ -5761,16 +5783,16 @@
         <v>22</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F31" s="6">
         <v>45853</v>
@@ -5779,35 +5801,35 @@
         <v>2025</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="N31" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="R31" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="O31" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="R31" s="2" t="s">
-        <v>299</v>
-      </c>
       <c r="S31" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
@@ -5824,7 +5846,7 @@
         <v>0</v>
       </c>
       <c r="AB31" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC31" s="2">
         <v>0</v>
@@ -5847,53 +5869,53 @@
         <v>22</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G32" s="6">
         <v>2025</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J32" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q32" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="S32" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="S32" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
@@ -5914,7 +5936,7 @@
         <v>8</v>
       </c>
       <c r="AB32" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AC32" s="2">
         <v>1</v>
@@ -5937,53 +5959,53 @@
         <v>22</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G33" s="6">
         <v>2024</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>23</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="T33" s="2"/>
       <c r="U33" s="2"/>
@@ -6004,7 +6026,7 @@
         <v>10</v>
       </c>
       <c r="AB33" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC33" s="2">
         <v>5</v>
@@ -6027,25 +6049,25 @@
         <v>22</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G34" s="6">
         <v>2023</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>19</v>
@@ -6055,25 +6077,25 @@
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O34" s="2" t="s">
         <v>21</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q34" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
@@ -6117,25 +6139,25 @@
         <v>22</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G35" s="6">
         <v>2022</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>19</v>
@@ -6145,25 +6167,25 @@
       </c>
       <c r="K35" s="2"/>
       <c r="L35" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="N35" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="R35" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="O35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="R35" s="2" t="s">
+      <c r="S35" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="S35" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
@@ -6207,53 +6229,53 @@
         <v>22</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G36" s="6">
         <v>2022</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N36" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="S36" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="S36" s="2" t="s">
-        <v>310</v>
       </c>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
@@ -6297,53 +6319,53 @@
         <v>22</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G37" s="6">
         <v>2021</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N37" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="S37" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="R37" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>314</v>
       </c>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
@@ -6387,53 +6409,53 @@
         <v>22</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G38" s="6">
         <v>2020</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I38" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="R38" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
@@ -6454,7 +6476,7 @@
         <v>93</v>
       </c>
       <c r="AB38" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC38" s="2">
         <v>31</v>
@@ -6477,53 +6499,53 @@
         <v>22</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G39" s="6">
         <v>2020</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
@@ -6544,7 +6566,7 @@
         <v>75</v>
       </c>
       <c r="AB39" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC39" s="2">
         <v>38</v>
@@ -6567,49 +6589,49 @@
         <v>22</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G40" s="6">
         <v>2020</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K40" s="2"/>
       <c r="L40" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N40" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P40" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q40" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>426</v>
       </c>
       <c r="R40" s="2"/>
       <c r="S40" s="2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
@@ -6630,7 +6652,7 @@
         <v>0</v>
       </c>
       <c r="AB40" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC40" s="2">
         <v>0</v>
@@ -6653,25 +6675,25 @@
         <v>22</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G41" s="6">
         <v>2019</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>19</v>
@@ -6681,25 +6703,25 @@
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="O41" s="2" t="s">
         <v>24</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q41" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
@@ -6743,51 +6765,51 @@
         <v>22</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G42" s="6">
         <v>2019</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J42" s="2" t="s">
         <v>23</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q42" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="R42" s="2"/>
       <c r="S42" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
@@ -6831,53 +6853,53 @@
         <v>22</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G43" s="6">
         <v>2018</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>30</v>
+        <v>579</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q43" s="7" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
@@ -6898,7 +6920,7 @@
         <v>139</v>
       </c>
       <c r="AB43" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AC43" s="2">
         <v>139</v>
@@ -6921,53 +6943,53 @@
         <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G44" s="6">
         <v>2018</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="N44" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q44" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="R44" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="O44" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="Q44" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="R44" s="2" t="s">
-        <v>431</v>
-      </c>
       <c r="S44" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
@@ -6988,7 +7010,7 @@
         <v>114</v>
       </c>
       <c r="AB44" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AC44" s="2">
         <v>57</v>
@@ -7011,53 +7033,53 @@
         <v>22</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G45" s="6">
         <v>2016</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K45" s="2"/>
       <c r="L45" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N45" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
@@ -7101,51 +7123,51 @@
         <v>22</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G46" s="6">
         <v>2016</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q46" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="R46" s="2"/>
       <c r="S46" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
@@ -7166,7 +7188,7 @@
         <v>6</v>
       </c>
       <c r="AB46" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AC46" s="2">
         <v>2</v>
@@ -7189,49 +7211,49 @@
         <v>22</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G47" s="6">
         <v>2016</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="R47" s="2"/>
       <c r="S47" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
@@ -7271,53 +7293,53 @@
         <v>22</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G48" s="6">
         <v>2015</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N48" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="R48" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="S48" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="O48" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q48" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="R48" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="S48" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
@@ -7361,53 +7383,53 @@
         <v>22</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G49" s="6">
         <v>2013</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N49" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="R49" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="O49" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q49" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="R49" s="2" t="s">
+      <c r="S49" s="2" t="s">
         <v>439</v>
-      </c>
-      <c r="S49" s="2" t="s">
-        <v>440</v>
       </c>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
@@ -7428,7 +7450,7 @@
         <v>9</v>
       </c>
       <c r="AB49" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AC49" s="2">
         <v>5</v>
@@ -7451,51 +7473,51 @@
         <v>22</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G50" s="6">
         <v>2013</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I50" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="J50" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="K50" s="2"/>
       <c r="L50" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N50" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="R50" s="2"/>
       <c r="S50" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
@@ -7516,7 +7538,7 @@
         <v>6</v>
       </c>
       <c r="AB50" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AC50" s="2">
         <v>3</v>
@@ -7539,25 +7561,25 @@
         <v>22</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G51" s="6">
         <v>2012</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>14</v>
@@ -7567,23 +7589,23 @@
       </c>
       <c r="K51" s="2"/>
       <c r="L51" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="O51" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q51" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="R51" s="2"/>
       <c r="S51" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
@@ -7619,51 +7641,51 @@
         <v>22</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G52" s="6">
         <v>2011</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I52" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J52" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="K52" s="2"/>
       <c r="L52" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="O52" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="P52" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="R52" s="2"/>
       <c r="S52" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
@@ -7704,53 +7726,53 @@
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G53" s="6">
         <v>2024</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I53" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J53" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="K53" s="2"/>
       <c r="L53" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M53" s="7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="O53" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P53" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="R53" s="2"/>
       <c r="S53" s="2"/>
@@ -7769,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="AB53" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC53" s="2">
         <v>1</v>
@@ -7789,58 +7811,58 @@
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G54" s="6">
         <v>2021</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K54" s="2"/>
       <c r="L54" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M54" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Q54" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="R54" s="2"/>
       <c r="S54" s="2"/>
       <c r="T54" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="U54" s="2"/>
       <c r="V54" s="2"/>
@@ -7876,51 +7898,51 @@
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G55" s="6">
         <v>2021</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I55" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J55" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="K55" s="2"/>
       <c r="L55" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="N55" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="O55" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P55" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="R55" s="2"/>
       <c r="S55" s="2"/>
@@ -7959,56 +7981,56 @@
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G56" s="6">
         <v>2017</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I56" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J56" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M56" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="R56" s="2"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="U56" s="2"/>
       <c r="V56" s="2"/>
@@ -8046,55 +8068,58 @@
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G57" s="6">
         <v>2015</v>
       </c>
       <c r="H57" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J57" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="I57" s="2" t="s">
+      <c r="K57" s="2"/>
+      <c r="L57" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="M57" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="O57" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J57" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="K57" s="2"/>
-      <c r="M57" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="N57" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="O57" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="P57" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="R57" s="2"/>
       <c r="S57" s="2"/>
       <c r="T57" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="U57" s="2"/>
       <c r="V57" s="2"/>
@@ -8126,51 +8151,51 @@
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G58" s="6">
         <v>2015</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K58" s="2"/>
       <c r="L58" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="N58" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P58" s="2"/>
       <c r="Q58" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
@@ -8189,7 +8214,7 @@
         <v>2</v>
       </c>
       <c r="AB58" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AC58" s="2">
         <v>1</v>
@@ -8209,53 +8234,53 @@
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G59" s="6">
         <v>2014</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K59" s="2"/>
       <c r="L59" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P59" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="Q59" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
@@ -8297,49 +8322,49 @@
         <v>17</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G60" s="6">
         <v>2016</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K60" s="2"/>
       <c r="N60" s="2"/>
       <c r="O60" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P60" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q60" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="R60" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="S60" s="2"/>
       <c r="T60" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="U60" s="2"/>
       <c r="V60" s="2"/>
@@ -8351,7 +8376,7 @@
         <v>153</v>
       </c>
       <c r="AB60" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC60" s="2">
         <v>153</v>
@@ -8374,51 +8399,51 @@
         <v>17</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G61" s="6">
         <v>2014</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="O61" s="2" t="s">
         <v>16</v>
       </c>
       <c r="P61" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q61" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="R61" s="7"/>
       <c r="S61" s="7"/>
       <c r="T61" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="U61" s="7"/>
       <c r="V61" s="2"/>
@@ -8450,44 +8475,44 @@
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F62" s="6" t="s">
+        <v>529</v>
+      </c>
+      <c r="G62" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="G62" s="6" t="s">
+      <c r="H62" s="2" t="s">
         <v>531</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>532</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K62" s="2"/>
       <c r="L62" s="2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
       <c r="Q62" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="R62" s="2"/>
       <c r="S62" s="2" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
@@ -8508,44 +8533,44 @@
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F63" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="G63" s="6" t="s">
         <v>536</v>
       </c>
-      <c r="G63" s="6" t="s">
-        <v>537</v>
-      </c>
       <c r="H63" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K63" s="2"/>
       <c r="L63" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
       <c r="Q63" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="R63" s="2"/>
       <c r="S63" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
@@ -8566,44 +8591,44 @@
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F64" s="6" t="s">
+        <v>540</v>
+      </c>
+      <c r="G64" s="6" t="s">
         <v>541</v>
       </c>
-      <c r="G64" s="6" t="s">
-        <v>542</v>
-      </c>
       <c r="H64" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I64" s="2"/>
       <c r="J64" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K64" s="2"/>
       <c r="L64" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
       <c r="Q64" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="R64" s="2"/>
       <c r="S64" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
@@ -8624,42 +8649,42 @@
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F65" s="6" t="s">
         <v>545</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="F65" s="6" t="s">
+      <c r="G65" s="6" t="s">
         <v>546</v>
       </c>
-      <c r="G65" s="6" t="s">
-        <v>547</v>
-      </c>
       <c r="H65" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I65" s="2"/>
       <c r="J65" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="K65" s="2"/>
       <c r="L65" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
       <c r="Q65" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="R65" s="2"/>
       <c r="S65" s="2"/>
@@ -8682,44 +8707,44 @@
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F66" s="6" t="s">
+        <v>551</v>
+      </c>
+      <c r="G66" s="6" t="s">
         <v>552</v>
       </c>
-      <c r="G66" s="6" t="s">
-        <v>553</v>
-      </c>
       <c r="H66" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K66" s="2"/>
       <c r="L66" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
       <c r="Q66" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="R66" s="2"/>
       <c r="S66" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
@@ -8740,44 +8765,44 @@
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I67" s="2"/>
       <c r="J67" s="8" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K67" s="2"/>
       <c r="L67" s="8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
       <c r="Q67" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="R67" s="2"/>
       <c r="S67" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="T67" s="2"/>
       <c r="U67" s="2"/>
@@ -8798,44 +8823,44 @@
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I68" s="2"/>
       <c r="J68" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K68" s="2"/>
       <c r="L68" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
       <c r="Q68" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="R68" s="2"/>
       <c r="S68" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="T68" s="2"/>
       <c r="U68" s="2"/>
@@ -8856,44 +8881,44 @@
     </row>
     <row r="69" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F69" s="6" t="s">
+        <v>565</v>
+      </c>
+      <c r="G69" s="6" t="s">
         <v>566</v>
       </c>
-      <c r="G69" s="6" t="s">
-        <v>567</v>
-      </c>
       <c r="H69" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I69" s="2"/>
       <c r="J69" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K69" s="2"/>
       <c r="L69" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
       <c r="Q69" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="R69" s="2"/>
       <c r="S69" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="T69" s="2"/>
       <c r="U69" s="2"/>
@@ -8914,44 +8939,44 @@
     </row>
     <row r="70" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F70" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="G70" s="6" t="s">
         <v>572</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="H70" s="2" t="s">
         <v>573</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>574</v>
       </c>
       <c r="I70" s="2"/>
       <c r="J70" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K70" s="2"/>
       <c r="L70" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
       <c r="Q70" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="R70" s="2"/>
       <c r="S70" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="T70" s="2"/>
       <c r="U70" s="2"/>

</xml_diff>